<commit_message>
revisão até a lição 15 concluída
</commit_message>
<xml_diff>
--- a/Rune/Relatório.xlsx
+++ b/Rune/Relatório.xlsx
@@ -59,40 +59,40 @@
     <t>Date</t>
   </si>
   <si>
-    <t>January</t>
-  </si>
-  <si>
-    <t>February</t>
-  </si>
-  <si>
-    <t>March</t>
-  </si>
-  <si>
-    <t>April</t>
-  </si>
-  <si>
-    <t>May</t>
-  </si>
-  <si>
-    <t>June</t>
-  </si>
-  <si>
-    <t>July</t>
-  </si>
-  <si>
-    <t>August</t>
-  </si>
-  <si>
-    <t>September</t>
-  </si>
-  <si>
-    <t>October</t>
-  </si>
-  <si>
-    <t>November</t>
-  </si>
-  <si>
-    <t>December</t>
+    <t>Janeiro</t>
+  </si>
+  <si>
+    <t>Fevereiro</t>
+  </si>
+  <si>
+    <t>Março</t>
+  </si>
+  <si>
+    <t>Abril</t>
+  </si>
+  <si>
+    <t>Maio</t>
+  </si>
+  <si>
+    <t>Junho</t>
+  </si>
+  <si>
+    <t>Julho</t>
+  </si>
+  <si>
+    <t>Agosto</t>
+  </si>
+  <si>
+    <t>Setembro</t>
+  </si>
+  <si>
+    <t>Outubro</t>
+  </si>
+  <si>
+    <t>Novembro</t>
+  </si>
+  <si>
+    <t>Dezembro</t>
   </si>
 </sst>
 </file>
@@ -343,40 +343,40 @@
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>January</c:v>
+                  <c:v>Janeiro</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>February</c:v>
+                  <c:v>Fevereiro</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>March</c:v>
+                  <c:v>Março</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>April</c:v>
+                  <c:v>Abril</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>May</c:v>
+                  <c:v>Maio</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>June</c:v>
+                  <c:v>Junho</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>July</c:v>
+                  <c:v>Julho</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>August</c:v>
+                  <c:v>Agosto</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>September</c:v>
+                  <c:v>Setembro</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>October</c:v>
+                  <c:v>Outubro</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>November</c:v>
+                  <c:v>Novembro</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>December</c:v>
+                  <c:v>Dezembro</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>

</xml_diff>